<commit_message>
Made sure new bookings are added to the database for the user
</commit_message>
<xml_diff>
--- a/DatabaseFiles/Database tables.xlsx
+++ b/DatabaseFiles/Database tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Muhsin Chaudhary\Documents\Alameda Hackathon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Muhsin Chaudhary\Documents\Alameda Hackathon\DatabaseFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A667071-D284-4894-8F5E-70FB8FCB64BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75271E55-DAF8-47E0-A62A-B03DF411CD43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3C530FC4-D90E-4AFE-947F-AA13674E13F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3C530FC4-D90E-4AFE-947F-AA13674E13F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Flight Info" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="791">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="790">
   <si>
     <t>Flight Number</t>
   </si>
@@ -2407,9 +2407,6 @@
   </si>
   <si>
     <t>ID</t>
-  </si>
-  <si>
-    <t>FlightID</t>
   </si>
 </sst>
 </file>
@@ -2795,7 +2792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5255ED-08EB-4597-9297-93CBE8A3AC55}">
   <dimension ref="A1:I577"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+    <sheetView zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -21254,8 +21251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFFAC64D-76F2-4597-BAB9-5807D79334CA}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21274,9 +21271,7 @@
       <c r="C1" s="1" t="s">
         <v>788</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>790</v>
-      </c>
+      <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
   </sheetData>

</xml_diff>